<commit_message>
draft before submission to Barcelona
</commit_message>
<xml_diff>
--- a/tables/ScoringCard.xlsx
+++ b/tables/ScoringCard.xlsx
@@ -70,7 +70,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -79,12 +79,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="11"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -94,14 +100,14 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -109,7 +115,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -117,41 +123,119 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -161,26 +245,53 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -200,6 +311,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffffff00"/>
     </indexedColors>
@@ -400,17 +512,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -438,10 +550,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -689,12 +801,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -981,7 +1093,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1009,10 +1121,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1263,7 +1375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1319,7 +1431,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="s" s="5">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s" s="5">
         <v>8</v>
@@ -1358,6 +1470,41 @@
       <c r="E5" t="s" s="5">
         <v>8</v>
       </c>
+    </row>
+    <row r="6" ht="15.35" customHeight="1">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" ht="15.35" customHeight="1">
+      <c r="A7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" ht="15.35" customHeight="1">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12"/>
+    </row>
+    <row r="9" ht="15.35" customHeight="1">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="12"/>
+    </row>
+    <row r="10" ht="15.35" customHeight="1">
+      <c r="A10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated scoring card table
</commit_message>
<xml_diff>
--- a/tables/ScoringCard.xlsx
+++ b/tables/ScoringCard.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tao/Dropbox/InfVar/tables/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0668BFD-C839-AC49-AD92-4BA07A8A18B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="15960" windowHeight="15440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
   <si>
     <t xml:space="preserve">Criteria </t>
   </si>
@@ -49,11 +58,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -62,12 +68,8 @@
     <font>
       <sz val="12"/>
       <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -241,59 +243,26 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+  <cellXfs count="17">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -302,25 +271,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffffff00"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -522,7 +551,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -541,7 +570,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -571,7 +600,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -597,7 +626,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -623,7 +652,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -649,7 +678,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -675,7 +704,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -701,7 +730,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -727,7 +756,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -753,7 +782,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -779,7 +808,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -792,9 +821,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -811,7 +846,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -830,7 +865,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -856,7 +891,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -882,7 +917,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -908,7 +943,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -934,7 +969,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -960,7 +995,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -986,7 +1021,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1012,7 +1047,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1038,7 +1073,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1064,7 +1099,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1077,9 +1112,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1093,7 +1134,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1112,7 +1153,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1142,7 +1183,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1168,7 +1209,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1194,7 +1235,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1220,7 +1261,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1246,7 +1287,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1272,7 +1313,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1298,7 +1339,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1324,7 +1365,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1350,7 +1391,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1363,143 +1404,152 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.6719" style="1" customWidth="1"/>
-    <col min="2" max="5" width="10.8516" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.8516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="40.6640625" style="1" customWidth="1"/>
+    <col min="2" max="6" width="10.83203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.35" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="3">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="4">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="5">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="5">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="15.35" customHeight="1">
-      <c r="A2" t="s" s="5">
+    <row r="2" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s" s="6">
+      <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s" s="5">
+      <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s" s="5">
+      <c r="D2" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s" s="5">
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="C4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" ht="15.35" customHeight="1">
-      <c r="A3" t="s" s="5">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s" s="5">
+    <row r="5" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s" s="5">
+      <c r="C5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s" s="5">
+      <c r="D5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s" s="5">
-        <v>8</v>
-      </c>
     </row>
-    <row r="4" ht="15.35" customHeight="1">
-      <c r="A4" t="s" s="5">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s" s="5">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s" s="5">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s" s="5">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" ht="15.35" customHeight="1">
-      <c r="A5" t="s" s="5">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s" s="5">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s" s="5">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s" s="5">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" ht="15.35" customHeight="1">
+    <row r="6" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="9"/>
     </row>
-    <row r="7" ht="15.35" customHeight="1">
+    <row r="7" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
     </row>
-    <row r="8" ht="15.35" customHeight="1">
+    <row r="8" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="12"/>
     </row>
-    <row r="9" ht="15.35" customHeight="1">
+    <row r="9" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
     </row>
-    <row r="10" ht="15.35" customHeight="1">
+    <row r="10" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
@@ -1508,7 +1558,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
updated new estimates table for the revised paper
</commit_message>
<xml_diff>
--- a/tables/ScoringCard.xlsx
+++ b/tables/ScoringCard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tao/Dropbox/InfVar/tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bocdaz-my.sharepoint.com/personal/want_bocdaz_ca/Documents/GitHub/InfVar/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0668BFD-C839-AC49-AD92-4BA07A8A18B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{E0668BFD-C839-AC49-AD92-4BA07A8A18B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E942C7D7-5DC6-4AA4-BE22-89129E5BFCB3}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="15960" windowHeight="15440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1426,17 +1426,17 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="40.6640625" style="1" customWidth="1"/>
     <col min="2" max="6" width="10.83203125" style="1" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1461,16 +1461,16 @@
         <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -1484,10 +1484,10 @@
         <v>8</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
@@ -1495,16 +1495,16 @@
         <v>6</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -1515,41 +1515,41 @@
         <v>8</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="9"/>
     </row>
-    <row r="7" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
     </row>
-    <row r="8" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="12"/>
     </row>
-    <row r="9" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
     </row>
-    <row r="10" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>

</xml_diff>